<commit_message>
Surface XML:IDs for spreadsheet submissions
</commit_message>
<xml_diff>
--- a/openn/tests/data/bibliophilly/FLPLewisE087/openn_metadata.xlsx
+++ b/openn/tests/data/bibliophilly/FLPLewisE087/openn_metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27240" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27240" windowHeight="14900" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -12899,7 +12899,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -12965,6 +12965,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -13407,6 +13408,57 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="9" name="Rectangle 23" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 23" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -13906,6 +13958,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1422400</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 6" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -14174,7 +14277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -42728,13 +42831,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG21"/>
+  <dimension ref="A1:AG22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4:C21"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -43364,6 +43467,11 @@
       <c r="M21" s="12"/>
       <c r="N21" s="7"/>
       <c r="O21" s="12"/>
+    </row>
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="51">
+        <v>139</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>